<commit_message>
Aktualisierung auf nur noch offene Ideen
</commit_message>
<xml_diff>
--- a/Dokumentationen/HS-Hof-App-Ideen.xlsx
+++ b/Dokumentationen/HS-Hof-App-Ideen.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekt\Mobile.AndroidStudio\Hof.Stundenplaner\GitHub.Android\Dokumentationen\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="252" windowWidth="23256" windowHeight="9672"/>
   </bookViews>
   <sheets>
     <sheet name="HS Hof Android App" sheetId="5" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'HS Hof Android App'!$A$1:$C$17</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Inhalt</t>
   </si>
@@ -31,9 +39,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>(x)</t>
-  </si>
-  <si>
     <t>(Bus-)fahrplan</t>
   </si>
   <si>
@@ -77,6 +82,9 @@
   </si>
   <si>
     <t>Lageplan/ Campusnavi (keine Raumnummern einzelner Personen)</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -369,14 +377,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -414,9 +425,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -451,7 +462,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -486,7 +497,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -660,10 +671,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -679,15 +691,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>4</v>
@@ -698,7 +710,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>4</v>
@@ -712,11 +724,13 @@
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>4</v>
@@ -734,25 +748,27 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="19"/>
+    </row>
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="19"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>4</v>
@@ -768,7 +784,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>4</v>
@@ -777,16 +793,16 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>4</v>
@@ -797,32 +813,32 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="27"/>
@@ -891,6 +907,11 @@
       <c r="B36" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C17">
+    <filterColumn colId="2">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:B42">
     <sortCondition ref="A2:A42"/>
   </sortState>

</xml_diff>